<commit_message>
POSTFIX: circular-rna use non-copyright image
</commit_message>
<xml_diff>
--- a/WWW/posts/circular-rnas/post_info.xlsx
+++ b/WWW/posts/circular-rnas/post_info.xlsx
@@ -5,124 +5,150 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="756" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
-  <si>
-    <t>The Dish on Science</t>
-  </si>
-  <si>
-    <t>Post Information</t>
-  </si>
-  <si>
-    <t>Instructions:</t>
-  </si>
-  <si>
-    <t>Please fill in the values column for each relevant field. Please leave all fields that you do not use BLANK. Submissions not following instructions in the Description column will be rejected.</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Fields</t>
-  </si>
-  <si>
-    <t>Values</t>
-  </si>
-  <si>
-    <t>100 character max (inc spaces)</t>
-  </si>
-  <si>
-    <t>Post Title</t>
-  </si>
-  <si>
-    <t>Circular RNAs…What Goes Around, Comes Around</t>
-  </si>
-  <si>
-    <t>100 character max, only lowercase letters and hyphens (NO SPACES!) This will be what comes after ...com/posts/ in your post's URL. Be descriptive, and separate words with hyphens.</t>
-  </si>
-  <si>
-    <t>Post URL</t>
-  </si>
-  <si>
-    <t>circular-rnas</t>
-  </si>
-  <si>
-    <t>./images/IMAGE_FILE_NAME (include the extension). Remember, this will be used as the title image for the article, so don’t include it again within the article. Make sure it represents the article well as a whole, since it will be the visual representation of your article on the site. Also, make sure that it is high enough resolution to look good when full-screened, since it will be very large at the top of your article.</t>
-  </si>
-  <si>
-    <t>5x2 (WxH) Image File Name</t>
-  </si>
-  <si>
-    <t>./images/Research-Figure-5.jpg</t>
-  </si>
-  <si>
-    <t>Post Blurb</t>
-  </si>
-  <si>
-    <t>The quest towards a well-rounded understanding of RNA</t>
-  </si>
-  <si>
-    <t>500 character max (inc spaces). Shorter is usually better. Aim for 200 characters.</t>
-  </si>
-  <si>
-    <t>Post Description</t>
-  </si>
-  <si>
-    <t>In the biological world, we see that many things come in different shapes and sizes: animals, plants, microbes, and proteins. It turns out that even RNA falls into that category. In this article, we will explore what circular RNAs are, the history of their discovery, and why we should care about them. </t>
-  </si>
-  <si>
-    <t>thedishonscience.stanford.edu/topics/USE-THIS-STRING</t>
-  </si>
-  <si>
-    <t>Team Name(s)</t>
-  </si>
-  <si>
-    <t>biochemistry-and-bioinformatics</t>
-  </si>
-  <si>
-    <t>Please use EXACTLY the same name each time you submit a new post. This is like your username. If there is more than one author, use one column per author.</t>
-  </si>
-  <si>
-    <t>Author Name(s)</t>
-  </si>
-  <si>
-    <t>Joy Wan</t>
-  </si>
-  <si>
-    <t>Only use this if you want to have a specific headshot just for this article. Otherwise, leave blank. By default the picture submitted with the author_info form will be used. Remember to fill out the author_info Excel form if you want a page on the website about yourself!</t>
-  </si>
-  <si>
-    <t>Author Headshot File Name(s)</t>
-  </si>
-  <si>
-    <t>Please use EXACTLY the same name each time you submit a new post. This is like your username.</t>
-  </si>
-  <si>
-    <t>Illustrator Name(s)</t>
-  </si>
-  <si>
-    <t>Illustrator Headshot File Name(s)</t>
-  </si>
-  <si>
-    <t>./images/IMAGE_FILE_NAME (include the extension). This should be a cropped version of your "5x2 (WxH) Image File" if possible. This will be used if your article makes it to the most popular list.</t>
-  </si>
-  <si>
-    <t>2x1 (WxH) Image File Name</t>
-  </si>
-  <si>
-    <t>./images/IMAGE_FILE_NAME (include the extension). This should be an image that looks good when it is very tiny, like 80px by 80px. This will be used as a thumbnail for your article when necessary, for example if someone shares your article on Facebook, this is what they'll see.</t>
-  </si>
-  <si>
-    <t>1x1 (WxH) Image File Name (Thumbnail)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+  <si>
+    <t xml:space="preserve">The Dish on Science</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Post Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instructions:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please fill in the values column for each relevant field. Please leave all fields that you do not use BLANK. Submissions not following instructions in the Description column will be rejected.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 character max (inc spaces)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Post Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Circular RNAs…What Goes Around, Comes Around</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://thedishonscience.stanford.edu/posts/THIS-STRING    (100 Character max, only lowercase letters and hyphens, NO SPACES!). Be descriptive, and separate words with hyphens. Short if possible!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Post URL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">circular-rnas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./images/IMAGE_FILE_NAME (include the extension). Remember, this will be used as the title image for the article, so don’t include it again within the article. Make sure it represents the article well as a whole, since it will be the visual representation of your article on the site. Also, make sure that it is high enough resolution to look good when full-screened, since it will be very large at the top of your article.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5x2 (WxH) Image File Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./images/circular-rna.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Post Blurb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The quest towards a well-rounded understanding of RNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">500 character max (inc spaces). Shorter is usually better. Aim for 200 characters.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Post Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the biological world, we see that many things come in different shapes and sizes: animals, plants, microbes, and proteins. It turns out that even RNA falls into that category. In this article, we will explore what circular RNAs are, the history of their discovery, and why we should care about them. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">thedishonscience.stanford.edu/topics/USE-THIS-STRING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team Name(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biochemistry-and-bioinformatics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please use EXACTLY the same name each time you submit a new post. This is like your username. If there is more than one author, use one column per author.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Author Name(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joy Wan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This will be the name that is actually displayed on the website. Readers will not see the “Author Name” field.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Author Nickname(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joy Y. Wan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only use this if you want to have a specific headshot just for this article. Otherwise, leave blank. By default the picture submitted with the author_info form will be used. Remember to fill out the author_info Excel form if you want a page on the website about yourself!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Author Headshot File Name(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please use EXACTLY the same name each time you submit a new post. This is like your username.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Illustrator Name(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This will be the name that is actually displayed on the website. Readers will not see the “Illustrator Name” field.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Illustrator Nickname(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Illustrator Headshot File Name(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./images/IMAGE_FILE_NAME (include the extension). This should be a cropped version of your "5x2 (WxH) Image File" if possible. This will be used if your article makes it to the most popular list.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2x1 (WxH) Image File Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./images/IMAGE_FILE_NAME (include the extension). This should be an image that looks good when it is very tiny, like 80px by 80px. This will be used as a thumbnail for your article when necessary, for example if someone shares your article on Facebook, this is what they'll see.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1x1 (WxH) Image File Name (Thumbnail)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is for use only by the Dish administration.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Publication Date</t>
   </si>
 </sst>
 </file>
@@ -130,7 +156,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
   <fonts count="11">
@@ -202,9 +228,11 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -361,7 +389,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -369,11 +397,11 @@
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -381,14 +409,6 @@
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="5" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -401,7 +421,15 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -413,7 +441,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Explanatory Text" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -488,10 +516,10 @@
       <xdr:rowOff>39600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>730800</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2160</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>216000</xdr:rowOff>
+      <xdr:rowOff>214920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -505,7 +533,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="119160" y="39600"/>
-          <a:ext cx="611640" cy="912960"/>
+          <a:ext cx="930600" cy="937080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -525,22 +553,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C14" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.165991902834"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="41.9959514170041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="34.336032388664"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="40.663967611336"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="2" width="8.83400809716599"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="47.2448979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="35.6377551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="62.6377551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="33.8826530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="2" width="8.23469387755102"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -551,7 +582,7 @@
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
     </row>
-    <row r="2" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3"/>
       <c r="B2" s="6" t="s">
         <v>1</v>
@@ -573,7 +604,7 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3"/>
       <c r="B4" s="9" t="s">
         <v>3</v>
@@ -584,16 +615,15 @@
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3"/>
-      <c r="B5" s="0"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3"/>
       <c r="B6" s="10" t="s">
         <v>4</v>
@@ -623,7 +653,7 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" customFormat="false" ht="56.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="56.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3"/>
       <c r="B8" s="15" t="s">
         <v>10</v>
@@ -631,14 +661,14 @@
       <c r="C8" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="17" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" customFormat="false" ht="121.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3"/>
       <c r="B9" s="12" t="s">
         <v>13</v>
@@ -646,7 +676,7 @@
       <c r="C9" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="14" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="5"/>
@@ -661,7 +691,7 @@
       <c r="C10" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="17" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="5"/>
@@ -676,7 +706,7 @@
       <c r="C11" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="14" t="s">
         <v>20</v>
       </c>
       <c r="E11" s="5"/>
@@ -691,10 +721,10 @@
       <c r="C12" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="19"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
@@ -709,11 +739,11 @@
       <c r="D13" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-    </row>
-    <row r="14" customFormat="false" ht="87" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+    </row>
+    <row r="14" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3"/>
       <c r="B14" s="12" t="s">
         <v>27</v>
@@ -721,72 +751,107 @@
       <c r="C14" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="17"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-    </row>
-    <row r="15" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D14" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+    </row>
+    <row r="15" customFormat="false" ht="87" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3"/>
-      <c r="B15" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="16" t="s">
+      <c r="B15" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-    </row>
-    <row r="16" customFormat="false" ht="84" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C15" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="14"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+    </row>
+    <row r="16" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3"/>
       <c r="B16" s="15" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-    </row>
-    <row r="17" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>33</v>
+      </c>
+      <c r="D16" s="17"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+    </row>
+    <row r="17" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3"/>
       <c r="B17" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>35</v>
       </c>
       <c r="D17" s="17"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-    </row>
-    <row r="18" customFormat="false" ht="81.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+    </row>
+    <row r="18" customFormat="false" ht="84" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="3"/>
       <c r="B18" s="15" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="19"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D19" s="22" t="n">
+        <v>36</v>
+      </c>
+      <c r="D18" s="17"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+    </row>
+    <row r="19" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3"/>
+      <c r="B19" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="14"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3"/>
+      <c r="B20" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="17"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" s="21" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="20"/>
+      <c r="B21" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="22" t="n">
         <v>42823</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>